<commit_message>
updated data for ICAP analysis
</commit_message>
<xml_diff>
--- a/Active Learning Repo.xlsx
+++ b/Active Learning Repo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeachBox\TeachBox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niki/Downloads/ILGC6Teach/TeachBox/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E0F69F-FB7D-B047-AF0F-B61F6335FF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20445" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automation &amp; Control Engineerin" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="193">
   <si>
     <t>Biomedical Engineering</t>
   </si>
@@ -378,9 +379,6 @@
     <t>The game has been used during three consecutive years in a Masters’ level course. Surveys and course evaluations were used to evaluate the effectiveness of this method from both teacher and student perspectives.</t>
   </si>
   <si>
-    <t>The results show that students gained knowledge on complex subjects, and both teachers and students had positive experiences. Better integration of the game within the rest of the course could strengthen its effectiveness.</t>
-  </si>
-  <si>
     <t>Hotle, S., &amp; Garrow, L. A. (2016). Effects of the Traditional and Flipped Classrooms on Undergraduate Student Opinions and Success. Journal of Professional Issues in Engineering Education and Practice, 142(1).</t>
   </si>
   <si>
@@ -406,9 +404,6 @@
   </si>
   <si>
     <t>The empirical experience described here confirms the positive impact of active learning methods and indicates the key factors, both intrinsic and extrinsic, in the motivation of aerospace engineering students.</t>
-  </si>
-  <si>
-    <t>S-C,S-S,S-T</t>
   </si>
   <si>
     <t>Game Based Learning</t>
@@ -690,16 +685,19 @@
     <t>ICA</t>
   </si>
   <si>
-    <t>Hybrid</t>
+    <t>The lecture sessions were conducted using the online google meet platform. A padlet wall, Google form and paper slips were created for the collection of Muddiest Points and responses to One Minute Paper</t>
   </si>
   <si>
-    <t>The lecture sessions were conducted using the online google meet platform. A padlet wall, Google form and paper slips were created for the collection of Muddiest Points and responses to One Minute Paper</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -778,10 +776,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -794,7 +792,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -809,8 +807,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1026,36 +1025,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:WWH40"/>
+  <dimension ref="A1:WWL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="41" style="7" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="7"/>
-    <col min="10" max="10" width="57.140625" style="7" customWidth="1"/>
-    <col min="11" max="15" width="12.5703125" style="7"/>
-    <col min="16" max="16" width="33.7109375" style="7" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="7"/>
+    <col min="8" max="8" width="30.6640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="7"/>
+    <col min="10" max="10" width="57.1640625" style="7" customWidth="1"/>
+    <col min="11" max="19" width="12.5" style="7"/>
+    <col min="20" max="20" width="33.6640625" style="7" customWidth="1"/>
+    <col min="21" max="16384" width="12.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>10</v>
@@ -1094,16 +1093,28 @@
         <v>21</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="180" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="180" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1114,22 +1125,22 @@
         <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>29</v>
@@ -1143,17 +1154,29 @@
       <c r="M2" s="3">
         <v>2</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="3">
+        <v>4</v>
+      </c>
+      <c r="O2" s="3">
+        <v>4</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>182</v>
+      <c r="S2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="159.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="159.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1164,10 +1187,10 @@
         <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>34</v>
@@ -1193,14 +1216,26 @@
       <c r="M3" s="3">
         <v>2</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="3">
+        <v>4</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1211,10 +1246,10 @@
         <v>40</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>80</v>
@@ -1237,17 +1272,29 @@
       <c r="M4" s="7">
         <v>2</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O4" s="6" t="s">
+      <c r="N4" s="7">
+        <v>3</v>
+      </c>
+      <c r="O4" s="7">
+        <v>3</v>
+      </c>
+      <c r="P4" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>189</v>
+      <c r="T4" s="6" t="s">
+        <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1261,22 +1308,22 @@
         <v>44</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="K5" s="1">
         <v>2</v>
@@ -1287,17 +1334,29 @@
       <c r="M5" s="1">
         <v>2</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="1">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>4</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1351,23 +1410,36 @@
       <c r="J7" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="K7" s="7">
+        <v>2</v>
+      </c>
       <c r="L7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="3">
         <v>1</v>
       </c>
       <c r="N7" s="3">
-        <v>2</v>
-      </c>
-      <c r="O7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="S7" s="11" t="s">
         <v>31</v>
       </c>
+      <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1386,8 +1458,35 @@
       <c r="J8" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="K8" s="7">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1406,8 +1505,35 @@
       <c r="H9" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="K9" s="7">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>4</v>
+      </c>
+      <c r="O9" s="3">
+        <v>4</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1432,8 +1558,35 @@
       <c r="J10" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="K10" s="7">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>4</v>
+      </c>
+      <c r="O10" s="3">
+        <v>4</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1446,8 +1599,35 @@
       <c r="F11" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="K11" s="7">
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <v>2</v>
+      </c>
+      <c r="N11" s="7">
+        <v>3</v>
+      </c>
+      <c r="O11" s="7">
+        <v>3</v>
+      </c>
+      <c r="P11" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>1</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1469,8 +1649,35 @@
       <c r="J12" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="K12" s="7">
+        <v>1</v>
+      </c>
+      <c r="L12" s="7">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <v>2</v>
+      </c>
+      <c r="N12" s="7">
+        <v>3</v>
+      </c>
+      <c r="O12" s="7">
+        <v>3</v>
+      </c>
+      <c r="P12" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>1</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" ht="164.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="164.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -1481,10 +1688,10 @@
         <v>40</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>41</v>
@@ -1498,14 +1705,26 @@
       <c r="M13" s="3">
         <v>2</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="3">
+        <v>4</v>
+      </c>
+      <c r="O13" s="3">
+        <v>4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="S13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1524,8 +1743,35 @@
       <c r="J14" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="K14" s="7">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7">
+        <v>2</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>4</v>
+      </c>
+      <c r="O14" s="7">
+        <v>1</v>
+      </c>
+      <c r="P14" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>1</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1544,8 +1790,35 @@
       <c r="H15" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
+        <v>2</v>
+      </c>
+      <c r="N15" s="7">
+        <v>3</v>
+      </c>
+      <c r="O15" s="7">
+        <v>3</v>
+      </c>
+      <c r="P15" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>1</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1561,8 +1834,35 @@
       <c r="I16" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="K16" s="7">
+        <v>1</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
+        <v>2</v>
+      </c>
+      <c r="N16" s="7">
+        <v>3</v>
+      </c>
+      <c r="O16" s="7">
+        <v>3</v>
+      </c>
+      <c r="P16" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>1</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="17" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1578,8 +1878,35 @@
       <c r="J17" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7">
+        <v>2</v>
+      </c>
+      <c r="N17" s="7">
+        <v>3</v>
+      </c>
+      <c r="O17" s="7">
+        <v>3</v>
+      </c>
+      <c r="P17" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>1</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1604,8 +1931,35 @@
       <c r="J18" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="K18" s="7">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
+        <v>2</v>
+      </c>
+      <c r="N18" s="7">
+        <v>3</v>
+      </c>
+      <c r="O18" s="7">
+        <v>3</v>
+      </c>
+      <c r="P18" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>1</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1618,8 +1972,35 @@
       <c r="F19" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="20" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1632,8 +2013,35 @@
       <c r="F20" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="21" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1662,26 +2070,34 @@
       <c r="J21" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K21"/>
+      <c r="K21">
+        <v>2</v>
+      </c>
       <c r="L21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M21" s="1">
         <v>1</v>
       </c>
       <c r="N21" s="1">
-        <v>2</v>
-      </c>
-      <c r="O21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="1">
+        <v>4</v>
+      </c>
+      <c r="P21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="S21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
+      <c r="T21" s="1"/>
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
@@ -17816,8 +18232,12 @@
       <c r="WWF21"/>
       <c r="WWG21"/>
       <c r="WWH21"/>
+      <c r="WWI21"/>
+      <c r="WWJ21"/>
+      <c r="WWK21"/>
+      <c r="WWL21"/>
     </row>
-    <row r="22" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
@@ -17844,26 +18264,33 @@
         <v>48</v>
       </c>
       <c r="J22"/>
-      <c r="K22"/>
+      <c r="K22" s="1">
+        <v>2</v>
+      </c>
       <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="7">
         <v>2</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
+        <v>4</v>
+      </c>
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1">
         <v>1</v>
       </c>
-      <c r="N22" s="1">
-        <v>2</v>
-      </c>
-      <c r="O22" s="1" t="s">
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
       <c r="U22"/>
       <c r="V22"/>
       <c r="W22"/>
@@ -33998,8 +34425,12 @@
       <c r="WWF22"/>
       <c r="WWG22"/>
       <c r="WWH22"/>
+      <c r="WWI22"/>
+      <c r="WWJ22"/>
+      <c r="WWK22"/>
+      <c r="WWL22"/>
     </row>
-    <row r="23" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
@@ -34020,15 +34451,33 @@
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
+      <c r="K23" s="1">
+        <v>2</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="N23" s="7">
+        <v>4</v>
+      </c>
+      <c r="O23" s="1">
+        <v>4</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="T23"/>
       <c r="U23"/>
       <c r="V23"/>
@@ -50164,8 +50613,12 @@
       <c r="WWF23"/>
       <c r="WWG23"/>
       <c r="WWH23"/>
+      <c r="WWI23"/>
+      <c r="WWJ23"/>
+      <c r="WWK23"/>
+      <c r="WWL23"/>
     </row>
-    <row r="24" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -50192,24 +50645,36 @@
       <c r="J24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K24"/>
+      <c r="K24" s="1">
+        <v>2</v>
+      </c>
       <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
         <v>2</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="7">
+        <v>4</v>
+      </c>
+      <c r="O24" s="1">
+        <v>4</v>
+      </c>
+      <c r="P24" s="1">
         <v>1</v>
       </c>
-      <c r="N24" s="1">
-        <v>2</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="S24" s="12" t="s">
         <v>31</v>
       </c>
+      <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
@@ -50230,16 +50695,36 @@
         <v>118</v>
       </c>
       <c r="J25"/>
-      <c r="K25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
+      <c r="K25" s="7">
+        <v>2</v>
+      </c>
+      <c r="L25" s="7">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
+        <v>4</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4</v>
+      </c>
+      <c r="P25" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>1</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T25"/>
     </row>
-    <row r="26" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
         <v>5</v>
       </c>
@@ -50253,19 +50738,41 @@
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
+      <c r="K26" s="12">
+        <v>1</v>
+      </c>
+      <c r="L26" s="12">
+        <v>1</v>
+      </c>
+      <c r="M26" s="12">
+        <v>2</v>
+      </c>
+      <c r="N26" s="12">
+        <v>4</v>
+      </c>
+      <c r="O26" s="12">
+        <v>4</v>
+      </c>
+      <c r="P26" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="12">
+        <v>1</v>
+      </c>
+      <c r="R26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T26"/>
     </row>
-    <row r="27" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -50279,10 +50786,10 @@
         <v>44</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -50297,43 +50804,77 @@
       <c r="M27" s="1">
         <v>2</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="N27" s="1">
+        <v>4</v>
+      </c>
+      <c r="O27" s="1">
+        <v>4</v>
+      </c>
+      <c r="P27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="D28"/>
       <c r="E28" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
-      <c r="P28"/>
+      <c r="K28" s="3">
+        <v>2</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3">
+        <v>2</v>
+      </c>
+      <c r="N28" s="3">
+        <v>4</v>
+      </c>
+      <c r="O28" s="3">
+        <v>4</v>
+      </c>
+      <c r="P28" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28"/>
     </row>
-    <row r="29" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -50345,85 +50886,151 @@
       </c>
       <c r="D29"/>
       <c r="E29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29"/>
       <c r="G29" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H29"/>
       <c r="I29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
+      <c r="K29" s="1">
+        <v>2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2</v>
+      </c>
+      <c r="N29" s="7">
+        <v>4</v>
+      </c>
+      <c r="O29" s="1">
+        <v>4</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="T29"/>
     </row>
-    <row r="30" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D30"/>
       <c r="E30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
+      <c r="K30" s="12">
+        <v>1</v>
+      </c>
+      <c r="L30" s="12">
+        <v>2</v>
+      </c>
+      <c r="M30" s="12">
+        <v>1</v>
+      </c>
+      <c r="N30" s="12">
+        <v>4</v>
+      </c>
+      <c r="O30" s="12">
+        <v>4</v>
+      </c>
+      <c r="P30" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="12">
+        <v>1</v>
+      </c>
+      <c r="R30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="31" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S31" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="32" spans="1:16154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -50450,89 +51057,147 @@
       <c r="J32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K32"/>
+      <c r="K32" s="1">
+        <v>2</v>
+      </c>
       <c r="L32" s="1">
+        <v>1</v>
+      </c>
+      <c r="M32" s="1">
         <v>2</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="7">
+        <v>4</v>
+      </c>
+      <c r="O32" s="1">
+        <v>4</v>
+      </c>
+      <c r="P32" s="1">
         <v>1</v>
       </c>
-      <c r="N32" s="1">
-        <v>2</v>
-      </c>
-      <c r="O32" s="1" t="s">
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="S32" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
+      <c r="K33" s="7">
+        <v>2</v>
+      </c>
+      <c r="L33" s="7">
+        <v>2</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1</v>
+      </c>
+      <c r="N33" s="7">
+        <v>4</v>
+      </c>
+      <c r="O33" s="7">
+        <v>1</v>
+      </c>
+      <c r="P33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>1</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T33"/>
     </row>
-    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
+      <c r="K34" s="7">
+        <v>2</v>
+      </c>
+      <c r="L34" s="7">
+        <v>2</v>
+      </c>
+      <c r="M34" s="7">
+        <v>1</v>
+      </c>
+      <c r="N34" s="7">
+        <v>4</v>
+      </c>
+      <c r="O34" s="7">
+        <v>1</v>
+      </c>
+      <c r="P34" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>1</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T34"/>
     </row>
-    <row r="35" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
@@ -50547,15 +51212,15 @@
       </c>
       <c r="E35"/>
       <c r="F35" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I35"/>
       <c r="J35" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K35" s="1">
         <v>2</v>
@@ -50566,22 +51231,34 @@
       <c r="M35" s="1">
         <v>2</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="N35" s="1">
+        <v>4</v>
+      </c>
+      <c r="O35" s="1">
+        <v>4</v>
+      </c>
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>72</v>
@@ -50589,32 +51266,52 @@
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="S36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T36" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O36"/>
-      <c r="P36" s="1" t="s">
-        <v>166</v>
-      </c>
     </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
@@ -50625,38 +51322,54 @@
         <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E37"/>
       <c r="F37" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K37"/>
-      <c r="L37" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M37"/>
-      <c r="N37" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="O37" s="1" t="s">
+      <c r="K37" s="12">
+        <v>1</v>
+      </c>
+      <c r="L37" s="12">
+        <v>1</v>
+      </c>
+      <c r="M37" s="12">
+        <v>2</v>
+      </c>
+      <c r="N37" s="12">
+        <v>4</v>
+      </c>
+      <c r="O37" s="12">
+        <v>4</v>
+      </c>
+      <c r="P37" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="12">
+        <v>1</v>
+      </c>
+      <c r="R37" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S37" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P37"/>
+      <c r="T37"/>
     </row>
-    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -50683,22 +51396,36 @@
       <c r="J38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K38"/>
+      <c r="K38" s="1">
+        <v>2</v>
+      </c>
       <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="M38" s="1">
         <v>2</v>
       </c>
-      <c r="M38" s="1">
+      <c r="N38" s="7">
+        <v>4</v>
+      </c>
+      <c r="O38" s="1">
+        <v>4</v>
+      </c>
+      <c r="P38" s="1">
         <v>1</v>
       </c>
-      <c r="N38" s="1">
-        <v>2</v>
-      </c>
-      <c r="O38" s="1" t="s">
+      <c r="Q38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P38"/>
+      <c r="S38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T38"/>
     </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
         <v>3</v>
       </c>
@@ -50716,60 +51443,104 @@
         <v>34</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
+      <c r="K39" s="1">
+        <v>2</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="1">
+        <v>2</v>
+      </c>
+      <c r="N39" s="1">
+        <v>4</v>
+      </c>
+      <c r="O39" s="1">
+        <v>4</v>
+      </c>
+      <c r="P39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>1</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39"/>
     </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
+      <c r="K40" s="3">
+        <v>2</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1</v>
+      </c>
+      <c r="M40" s="3">
+        <v>2</v>
+      </c>
+      <c r="N40" s="3">
+        <v>4</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4</v>
+      </c>
+      <c r="P40" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S40" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T40"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="G25" r:id="rId2"/>
-    <hyperlink ref="E30" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F34" r:id="rId5"/>
-    <hyperlink ref="F35" r:id="rId6"/>
-    <hyperlink ref="E2" r:id="rId7" location="muddiest-point"/>
-    <hyperlink ref="E5" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F34" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F35" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E2" r:id="rId7" location="muddiest-point" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>